<commit_message>
Save graph and image files for June, 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_y_graph.xlsx
+++ b/statistics_files/2024/2024_99_y_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2588676-0FFA-4439-A218-2EA5FA472A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65089E5-E2E9-46D8-99B5-4674449057D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,7 +1057,10 @@
                   <c:v>85725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106482</c:v>
+                  <c:v>93775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>106428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2142,7 +2145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2266,7 +2271,7 @@
         <v>95894</v>
       </c>
       <c r="F6">
-        <v>106482</v>
+        <v>93775</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2284,6 +2289,9 @@
       </c>
       <c r="E7">
         <v>114493</v>
+      </c>
+      <c r="F7">
+        <v>106428</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update images and some of the next files
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_y_graph.xlsx
+++ b/statistics_files/2024/2024_99_y_graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65089E5-E2E9-46D8-99B5-4674449057D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010FCF8-A767-4250-B5A6-EBD29CE82AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1061,6 +1061,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>106428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2146,15 +2149,15 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>83661</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>84080</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>89067</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>85725</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>93775</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>106428</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2310,8 +2313,11 @@
       <c r="E8">
         <v>101818</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>107365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>98924</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>89740</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>89776</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2379,7 +2385,7 @@
         <v>84962</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>75603</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2406,7 +2412,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2414,7 +2420,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2422,7 +2428,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2430,7 +2436,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2438,7 +2444,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2446,7 +2452,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2454,7 +2460,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2462,7 +2468,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2470,7 +2476,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2478,7 +2484,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2486,7 +2492,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2494,7 +2500,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2502,7 +2508,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2510,7 +2516,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
Updates for August 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_y_graph.xlsx
+++ b/statistics_files/2024/2024_99_y_graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010FCF8-A767-4250-B5A6-EBD29CE82AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4E6203-FAB3-439A-929F-D63F08726AE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1064,6 +1064,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>107365</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2149,15 +2152,15 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.69140625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>83661</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>84080</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>89067</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>85725</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>93775</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>106428</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>107365</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2333,8 +2336,11 @@
       <c r="E9">
         <v>98924</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F9">
+        <v>93549</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>89740</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2368,7 +2374,7 @@
         <v>89776</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>84962</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2408,7 @@
         <v>75603</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2412,7 +2418,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2420,7 +2426,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2428,7 +2434,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2436,7 +2442,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2444,7 +2450,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2452,7 +2458,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2460,7 +2466,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2468,7 +2474,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2476,7 +2482,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2484,7 +2490,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2492,7 +2498,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2500,7 +2506,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2508,7 +2514,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2516,7 +2522,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>

<commit_message>
Update all statistic files for September, 2024
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_y_graph.xlsx
+++ b/statistics_files/2024/2024_99_y_graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4E6203-FAB3-439A-929F-D63F08726AE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA09C2-E13A-486A-8285-948037CEE703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1067,6 +1067,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>93549</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83710</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,15 +2155,15 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>83661</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>84080</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>89067</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>85725</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2280,7 +2283,7 @@
         <v>93775</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>106428</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>107365</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2340,7 +2343,7 @@
         <v>93549</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2356,8 +2359,11 @@
       <c r="E10">
         <v>89740</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>83710</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>89776</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2391,7 +2397,7 @@
         <v>84962</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>75603</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2418,7 +2424,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2426,7 +2432,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2434,7 +2440,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2442,7 +2448,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2450,7 +2456,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2458,7 +2464,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2466,7 +2472,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2474,7 +2480,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2482,7 +2488,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2490,7 +2496,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2498,7 +2504,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2506,7 +2512,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2514,7 +2520,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2522,7 +2528,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>